<commit_message>
harmonisation oignons et tomates ok
</commit_message>
<xml_diff>
--- a/ingredients.xlsx
+++ b/ingredients.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renau\Convertisseur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE17E1C1-E180-4D0E-89AA-E5B816E70886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AD633E6-452D-4254-9328-5E564DEAE688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BB65F6B7-6B5B-4AD1-B2B4-57BEF641AB97}"/>
   </bookViews>
@@ -3754,11 +3754,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C99BCBC-C19B-4075-AB48-0622208F227E}">
   <dimension ref="A1:IL323"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="9" ySplit="14" topLeftCell="GY15" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="9" ySplit="14" topLeftCell="EW183" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomRight" activeCell="FF196" sqref="FF196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8423,6 +8423,15 @@
       <c r="EX191" t="s">
         <v>503</v>
       </c>
+      <c r="FB191">
+        <v>3</v>
+      </c>
+      <c r="FD191">
+        <v>2</v>
+      </c>
+      <c r="FF191">
+        <v>1</v>
+      </c>
     </row>
     <row r="192" spans="1:162" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
@@ -8505,6 +8514,15 @@
       </c>
       <c r="EX195" t="s">
         <v>511</v>
+      </c>
+      <c r="FB195">
+        <v>3</v>
+      </c>
+      <c r="FD195">
+        <v>1</v>
+      </c>
+      <c r="FF195">
+        <v>3</v>
       </c>
     </row>
     <row r="196" spans="1:173" x14ac:dyDescent="0.3">

</xml_diff>